<commit_message>
debug from csv  and  update sort rank logic
</commit_message>
<xml_diff>
--- a/data/RC_Category_2020_feature_word_to_low_vr2.xlsx
+++ b/data/RC_Category_2020_feature_word_to_low_vr2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacky Wang\Desktop\sg_recommend_systrm_for_api\function2_api_format\function2\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacky Wang\Desktop\git_lab_smart_guard\2020_7_4\six_sigma_kse\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5A842A2-C085-41A0-8F84-F724205EDCF7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF487E84-4EE4-45E0-A954-4E142BEEAED3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5A8C67EF-D718-40B1-912F-89EFCC993556}"/>
   </bookViews>
@@ -20,11 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -954,10 +949,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>不按照,按照,不遵守,validation,regular,宣導,私自,小過,學習,未鎖,未裝,自行,未使用,按sop,要求,漏鎖,規範,動作,稽核,漏銅,未檢,稽查,漏失,貼反,忘記,未帶,必須,用錯,打瞌睡,不集中,粗心,人為,陷阱,擺放,漏裝,不熟練,未黏貼,檢討,不小心,不會區分,紀律,誤將,自認為,未發現,漏撕,錯拿,疏忽,嚴格,警告,未認真,沒有按,懲處,誤判,手法,小過,手指,精神狀態,擺放,單手作業,大過,未確認,執行力,違背,人為,裝錯,傳閱,不當,自主,原則,糾正,提醒,手壓,手,輕拿,輕放,員工,疏忽,培訓,及時,要求,教導,自檢,品質意識,漏寫,沒有將,理解不夠,學習,未在,混放,審核,未將,簽名,未確認,不允許,品質意識不足,訓練,糾正,隨手,亂放,標識,臨時,加班,簽字,補簽,誤漏,較慢,trained,按照,未按照,嚴格,follow,followed,folminor,operator,improper,不一致,打開,開啟,調取,確認,需要,圖片不清晰,未用,discipline,don't,didn't,without,immediately,stricktly,mistake,in time,carefully,personnel,request,retrained,retrain,Technologis,aware of,must,execution,forgot,misalignment,right away,reaffirm,request,infracted,improperly</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>thernet</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2886,6 +2877,10 @@
   </si>
   <si>
     <t>監督,瞭解員工,關心員工,帶領,主管,行政處分,要求線長,不熟悉,及時,上報,未在,書寫不清,反饋,線長必須,線長,誤漏,宣導,line leader,smt leader,supervisor,manager</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不按照,按照,不遵守,validation,regular,宣導,私自,小過,學習,未鎖,未裝,自行,未使用,按sop,要求,漏鎖,規範,動作,稽核,漏銅,未檢,稽查,漏失,貼反,忘記,未帶,必須,用錯,打瞌睡,不集中,粗心,人為,陷阱,擺放,漏裝,不熟練,未黏貼,檢討,不小心,不會區分,紀律,誤將,自認為,未發現,漏撕,錯拿,疏忽,嚴格,警告,未認真,沒有按,懲處,誤判,手法,小過,手指,精神狀態,擺放,單手作業,大過,未確認,執行力,違背,人為,裝錯,傳閱,不當,自主,原則,糾正,提醒,手壓,手,輕拿,輕放,員工,疏忽,培訓,及時,要求,教導,自檢,品質意識,漏寫,沒有將,理解不夠,學習,未在,混放,審核,未將,簽名,未確認,不允許,品質意識不足,訓練,糾正,隨手,亂放,標識,臨時,加班,簽字,補簽,誤漏,較慢,trained,按照,未按照,嚴格,follow,followed,folminor,operator,improper,不一致,打開,開啟,調取,確認,需要,圖片不清晰,未用,discipline,don't,didn't,without,immediately,stricktly,mistake,in time,carefully,personnel,request,retrained,retrain,Technologis,aware of,must,execution,forgot,misalignment,right away,reaffirm,request,infracted,improperly,OP,qualification</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3359,8 +3354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{483B88D9-096B-4CE8-9E3A-CE6F3AD6F55C}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -3410,7 +3405,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="209.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3421,7 +3416,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3443,10 +3438,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" t="s">
         <v>35</v>
-      </c>
-      <c r="E7" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="126.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3468,7 +3463,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3479,7 +3474,7 @@
         <v>7</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="66.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3523,7 +3518,7 @@
         <v>11</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3567,7 +3562,7 @@
         <v>15</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="81.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3578,7 +3573,7 @@
         <v>16</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>